<commit_message>
update metdata and cw table
</commit_message>
<xml_diff>
--- a/Tables/PropertyRegistry.xlsx
+++ b/Tables/PropertyRegistry.xlsx
@@ -921,13 +921,13 @@
     <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7010</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/1730</t>
+  </si>
+  <si>
     <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6797</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6810</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/1730</t>
   </si>
   <si>
     <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6801</t>
@@ -17744,7 +17744,7 @@
         <v>50</v>
       </c>
       <c r="B75" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C75" t="s">
         <v>296</v>
@@ -17755,7 +17755,7 @@
         <v>50</v>
       </c>
       <c r="B76" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C76" t="s">
         <v>297</v>
@@ -17766,7 +17766,7 @@
         <v>50</v>
       </c>
       <c r="B77" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C77" t="s">
         <v>298</v>
@@ -17777,18 +17777,18 @@
         <v>50</v>
       </c>
       <c r="B78" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C78" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B79" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="C79" t="s">
         <v>298</v>
@@ -17799,10 +17799,10 @@
         <v>51</v>
       </c>
       <c r="B80" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="C80" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="81">
@@ -17810,10 +17810,10 @@
         <v>51</v>
       </c>
       <c r="B81" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="C81" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="82">
@@ -17821,10 +17821,10 @@
         <v>51</v>
       </c>
       <c r="B82" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C82" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="83">
@@ -17832,10 +17832,10 @@
         <v>51</v>
       </c>
       <c r="B83" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C83" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="84">
@@ -17843,10 +17843,10 @@
         <v>51</v>
       </c>
       <c r="B84" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C84" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="85">
@@ -17854,7 +17854,7 @@
         <v>51</v>
       </c>
       <c r="B85" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C85" t="s">
         <v>298</v>
@@ -17865,21 +17865,21 @@
         <v>51</v>
       </c>
       <c r="B86" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C86" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B87" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="C87" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="88">
@@ -17887,10 +17887,10 @@
         <v>52</v>
       </c>
       <c r="B88" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="C88" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="89">
@@ -17898,10 +17898,10 @@
         <v>52</v>
       </c>
       <c r="B89" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="C89" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="90">
@@ -17909,43 +17909,43 @@
         <v>52</v>
       </c>
       <c r="B90" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="C90" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B91" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C91" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B92" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="C92" t="s">
-        <v>296</v>
+        <v>258</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B93" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C93" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="94">
@@ -17953,43 +17953,43 @@
         <v>53</v>
       </c>
       <c r="B94" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="C94" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B95" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="C95" t="s">
-        <v>258</v>
+        <v>298</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B96" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="C96" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B97" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C97" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="98">
@@ -17997,10 +17997,10 @@
         <v>54</v>
       </c>
       <c r="B98" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="C98" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="99">
@@ -18008,10 +18008,10 @@
         <v>54</v>
       </c>
       <c r="B99" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="C99" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="100">
@@ -18019,43 +18019,43 @@
         <v>54</v>
       </c>
       <c r="B100" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="C100" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B101" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C101" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B102" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="C102" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B103" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C103" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="104">
@@ -18063,43 +18063,43 @@
         <v>55</v>
       </c>
       <c r="B104" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="C104" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B105" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
       <c r="C105" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B106" t="s">
-        <v>246</v>
+        <v>264</v>
       </c>
       <c r="C106" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B107" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C107" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="108">
@@ -18107,10 +18107,10 @@
         <v>56</v>
       </c>
       <c r="B108" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="C108" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="109">
@@ -18118,10 +18118,10 @@
         <v>56</v>
       </c>
       <c r="B109" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C109" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="110">
@@ -18129,43 +18129,43 @@
         <v>56</v>
       </c>
       <c r="B110" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="C110" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B111" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C111" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B112" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C112" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B113" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C113" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="114">
@@ -18173,43 +18173,43 @@
         <v>57</v>
       </c>
       <c r="B114" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="C114" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B115" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C115" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B116" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C116" t="s">
-        <v>303</v>
+        <v>258</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B117" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C117" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="118">
@@ -18217,51 +18217,51 @@
         <v>58</v>
       </c>
       <c r="B118" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C118" t="s">
-        <v>306</v>
+        <v>258</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B119" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C119" t="s">
-        <v>258</v>
+        <v>308</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B120" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C120" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B121" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="C121" t="s">
-        <v>258</v>
+        <v>308</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B122" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C122" t="s">
         <v>308</v>
@@ -18269,13 +18269,13 @@
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B123" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C123" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="124">
@@ -18283,18 +18283,18 @@
         <v>60</v>
       </c>
       <c r="B124" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="C124" t="s">
-        <v>308</v>
+        <v>258</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B125" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C125" t="s">
         <v>308</v>
@@ -18302,24 +18302,24 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B126" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C126" t="s">
-        <v>309</v>
+        <v>258</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B127" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C127" t="s">
-        <v>258</v>
+        <v>310</v>
       </c>
     </row>
     <row r="128">
@@ -18327,43 +18327,43 @@
         <v>61</v>
       </c>
       <c r="B128" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="C128" t="s">
-        <v>308</v>
+        <v>258</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B129" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C129" t="s">
-        <v>258</v>
+        <v>308</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B130" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C130" t="s">
-        <v>310</v>
+        <v>258</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B131" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C131" t="s">
-        <v>258</v>
+        <v>310</v>
       </c>
     </row>
     <row r="132">
@@ -18371,75 +18371,42 @@
         <v>62</v>
       </c>
       <c r="B132" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="C132" t="s">
-        <v>308</v>
+        <v>258</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B133" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C133" t="s">
-        <v>258</v>
+        <v>311</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B134" t="s">
         <v>251</v>
       </c>
       <c r="C134" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B135" t="s">
         <v>253</v>
       </c>
       <c r="C135" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="n">
-        <v>63</v>
-      </c>
-      <c r="B136" t="s">
-        <v>246</v>
-      </c>
-      <c r="C136" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="n">
-        <v>63</v>
-      </c>
-      <c r="B137" t="s">
-        <v>251</v>
-      </c>
-      <c r="C137" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="n">
-        <v>63</v>
-      </c>
-      <c r="B138" t="s">
-        <v>253</v>
-      </c>
-      <c r="C138" t="s">
         <v>258</v>
       </c>
     </row>

</xml_diff>